<commit_message>
summary updated with real dataset data corrected
</commit_message>
<xml_diff>
--- a/xfer_cksum_pipeline_summary.xlsx
+++ b/xfer_cksum_pipeline_summary.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35160" windowHeight="20740" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="082016" sheetId="9" r:id="rId1"/>
+    <sheet name="082316" sheetId="10" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,7 +572,6 @@
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -1560,29 +1559,29 @@
       </c>
       <c r="G15" s="1">
         <f>AVERAGE(J15:N15)</f>
-        <v>679.8</v>
+        <v>670.8</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="1"/>
-        <v>679.8</v>
+        <v>670.8</v>
       </c>
       <c r="J15" s="1">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="K15" s="1">
-        <v>679</v>
+        <v>669</v>
       </c>
       <c r="L15" s="1">
-        <v>682</v>
+        <v>670</v>
       </c>
       <c r="M15" s="2">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="N15" s="2">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="O15" s="1">
         <v>573</v>
@@ -1632,29 +1631,29 @@
       </c>
       <c r="G16" s="1">
         <f>AVERAGE(J16:N16)</f>
-        <v>481.4</v>
+        <v>545.6</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="1"/>
-        <v>481.4</v>
+        <v>545.6</v>
       </c>
       <c r="J16" s="1">
-        <v>478</v>
+        <v>541</v>
       </c>
       <c r="K16" s="1">
-        <v>482</v>
+        <v>543</v>
       </c>
       <c r="L16" s="1">
-        <v>482</v>
+        <v>548</v>
       </c>
       <c r="M16" s="2">
-        <v>482</v>
+        <v>548</v>
       </c>
       <c r="N16" s="2">
-        <v>483</v>
+        <v>548</v>
       </c>
       <c r="O16" s="1">
         <v>616</v>
@@ -1704,29 +1703,29 @@
       </c>
       <c r="G17" s="1">
         <f t="shared" ref="G17:G20" si="4">AVERAGE(J17:N17)</f>
-        <v>695</v>
+        <v>661.8</v>
       </c>
       <c r="H17" s="1">
         <v>174.75</v>
       </c>
       <c r="I17" s="1">
         <f>G17-H17</f>
-        <v>520.25</v>
+        <v>487.04999999999995</v>
       </c>
       <c r="J17" s="1">
-        <v>724</v>
+        <v>623</v>
       </c>
       <c r="K17" s="1">
-        <v>698</v>
+        <v>670</v>
       </c>
       <c r="L17" s="1">
-        <v>688</v>
+        <v>672</v>
       </c>
       <c r="M17" s="2">
-        <v>689</v>
+        <v>673</v>
       </c>
       <c r="N17" s="2">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="O17" s="1">
         <v>683</v>
@@ -1776,29 +1775,29 @@
       </c>
       <c r="G18" s="1">
         <f t="shared" si="4"/>
-        <v>597.20000000000005</v>
+        <v>569.20000000000005</v>
       </c>
       <c r="H18" s="1">
         <v>86.7</v>
       </c>
       <c r="I18" s="1">
         <f>G18-H18</f>
-        <v>510.50000000000006</v>
+        <v>482.50000000000006</v>
       </c>
       <c r="J18" s="1">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="K18" s="1">
-        <v>600</v>
+        <v>577</v>
       </c>
       <c r="L18" s="1">
-        <v>599</v>
+        <v>570</v>
       </c>
       <c r="M18" s="2">
-        <v>642</v>
+        <v>570</v>
       </c>
       <c r="N18" s="2">
-        <v>584</v>
+        <v>571</v>
       </c>
       <c r="O18" s="1">
         <v>385</v>
@@ -1848,29 +1847,29 @@
       </c>
       <c r="G19" s="1">
         <f t="shared" si="4"/>
-        <v>537.79999999999995</v>
+        <v>531.4</v>
       </c>
       <c r="H19" s="1">
         <v>13.2</v>
       </c>
       <c r="I19" s="1">
         <f>G19-H19</f>
-        <v>524.59999999999991</v>
+        <v>518.19999999999993</v>
       </c>
       <c r="J19" s="1">
+        <v>534</v>
+      </c>
+      <c r="K19" s="1">
+        <v>536</v>
+      </c>
+      <c r="L19" s="1">
+        <v>528</v>
+      </c>
+      <c r="M19" s="2">
         <v>529</v>
       </c>
-      <c r="K19" s="1">
-        <v>537</v>
-      </c>
-      <c r="L19" s="1">
-        <v>539</v>
-      </c>
-      <c r="M19" s="2">
-        <v>545</v>
-      </c>
       <c r="N19" s="2">
-        <v>539</v>
+        <v>530</v>
       </c>
       <c r="O19" s="1">
         <v>303</v>
@@ -1920,29 +1919,29 @@
       </c>
       <c r="G20" s="1">
         <f t="shared" si="4"/>
-        <v>526.20000000000005</v>
+        <v>542.20000000000005</v>
       </c>
       <c r="H20" s="1">
         <v>4.8</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" ref="I20:I38" si="5">G20-H20</f>
-        <v>521.40000000000009</v>
+        <v>537.40000000000009</v>
       </c>
       <c r="J20" s="1">
-        <v>522</v>
+        <v>543</v>
       </c>
       <c r="K20" s="1">
-        <v>526</v>
+        <v>543</v>
       </c>
       <c r="L20" s="1">
-        <v>528</v>
+        <v>539</v>
       </c>
       <c r="M20" s="2">
-        <v>528</v>
+        <v>542</v>
       </c>
       <c r="N20" s="2">
-        <v>527</v>
+        <v>544</v>
       </c>
       <c r="O20" s="1">
         <v>296</v>
@@ -2520,23 +2519,23 @@
       </c>
       <c r="G33" s="3">
         <f t="shared" si="6"/>
-        <v>2375</v>
+        <v>2382</v>
       </c>
       <c r="H33" s="1">
         <v>0</v>
       </c>
       <c r="I33" s="1">
         <f t="shared" si="5"/>
-        <v>2375</v>
+        <v>2382</v>
       </c>
       <c r="J33" s="3">
-        <v>2374</v>
+        <v>2372</v>
       </c>
       <c r="K33" s="3">
-        <v>2375</v>
+        <v>2393</v>
       </c>
       <c r="L33" s="3">
-        <v>2376</v>
+        <v>2381</v>
       </c>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
@@ -2564,23 +2563,23 @@
       </c>
       <c r="G34" s="3">
         <f t="shared" si="6"/>
-        <v>1670.3333333333333</v>
+        <v>1983.3333333333333</v>
       </c>
       <c r="H34" s="1">
         <v>0</v>
       </c>
       <c r="I34" s="1">
         <f t="shared" si="5"/>
-        <v>1670.3333333333333</v>
+        <v>1983.3333333333333</v>
       </c>
       <c r="J34" s="3">
-        <v>1669</v>
+        <v>1988</v>
       </c>
       <c r="K34" s="3">
-        <v>1672</v>
+        <v>1982</v>
       </c>
       <c r="L34" s="3">
-        <v>1670</v>
+        <v>1980</v>
       </c>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
@@ -2608,23 +2607,23 @@
       </c>
       <c r="G35" s="3">
         <f t="shared" si="6"/>
-        <v>2090</v>
+        <v>2097</v>
       </c>
       <c r="H35" s="1">
         <v>349.5</v>
       </c>
       <c r="I35" s="1">
         <f>G35-H35</f>
-        <v>1740.5</v>
+        <v>1747.5</v>
       </c>
       <c r="J35" s="3">
-        <v>2106</v>
+        <v>2086</v>
       </c>
       <c r="K35" s="3">
-        <v>2090</v>
+        <v>2095</v>
       </c>
       <c r="L35" s="3">
-        <v>2074</v>
+        <v>2110</v>
       </c>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
@@ -2652,23 +2651,23 @@
       </c>
       <c r="G36" s="3">
         <f t="shared" si="6"/>
-        <v>1927.6666666666667</v>
+        <v>1920</v>
       </c>
       <c r="H36" s="1">
         <v>173.4</v>
       </c>
       <c r="I36" s="1">
         <f t="shared" si="5"/>
-        <v>1754.2666666666667</v>
+        <v>1746.6</v>
       </c>
       <c r="J36" s="3">
-        <v>1949</v>
+        <v>1921</v>
       </c>
       <c r="K36" s="3">
         <v>1916</v>
       </c>
       <c r="L36" s="3">
-        <v>1918</v>
+        <v>1923</v>
       </c>
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
@@ -2696,23 +2695,23 @@
       </c>
       <c r="G37" s="3">
         <f t="shared" si="6"/>
-        <v>1811.3333333333333</v>
+        <v>1844.3333333333333</v>
       </c>
       <c r="H37" s="1">
         <v>26.4</v>
       </c>
       <c r="I37" s="1">
         <f t="shared" si="5"/>
-        <v>1784.9333333333332</v>
+        <v>1817.9333333333332</v>
       </c>
       <c r="J37" s="3">
-        <v>1821</v>
+        <v>1838</v>
       </c>
       <c r="K37" s="3">
-        <v>1804</v>
+        <v>1844</v>
       </c>
       <c r="L37" s="3">
-        <v>1809</v>
+        <v>1851</v>
       </c>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
@@ -2740,23 +2739,23 @@
       </c>
       <c r="G38" s="3">
         <f t="shared" si="6"/>
-        <v>1848.3333333333333</v>
+        <v>1948.3333333333333</v>
       </c>
       <c r="H38" s="1">
         <v>9.6</v>
       </c>
       <c r="I38" s="1">
         <f t="shared" si="5"/>
-        <v>1838.7333333333333</v>
+        <v>1938.7333333333333</v>
       </c>
       <c r="J38" s="3">
-        <v>1841</v>
+        <v>1935</v>
       </c>
       <c r="K38" s="3">
-        <v>1839</v>
+        <v>1930</v>
       </c>
       <c r="L38" s="3">
-        <v>1865</v>
+        <v>1980</v>
       </c>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>

</xml_diff>